<commit_message>
Fix tool list entry methods
</commit_message>
<xml_diff>
--- a/Data/ShopToolsList.xlsx
+++ b/Data/ShopToolsList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\FinishedShopApp\venv\TempSource\Service\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tesla/PycharmProjects/ShopMonitor_1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1851D16C-7D4C-4A38-BF5A-A2949FF46D05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15795CB3-166A-0443-95DE-80A698CEF168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CEA7B18F-0EDF-4F76-84FF-B52E9CA7BF6C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17880" windowHeight="22400" xr2:uid="{CEA7B18F-0EDF-4F76-84FF-B52E9CA7BF6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="102">
   <si>
     <t>#</t>
   </si>
@@ -135,7 +135,211 @@
     <t>Starrett-Calipers</t>
   </si>
   <si>
-    <t>Standard-Wrench_open-end</t>
+    <t>11/16</t>
+  </si>
+  <si>
+    <t>9/16</t>
+  </si>
+  <si>
+    <t>5/8</t>
+  </si>
+  <si>
+    <t>Standard-Wrench-open-end</t>
+  </si>
+  <si>
+    <t>Standard-Wrench-combination</t>
+  </si>
+  <si>
+    <t>3/4</t>
+  </si>
+  <si>
+    <t>13/16</t>
+  </si>
+  <si>
+    <t>15/16</t>
+  </si>
+  <si>
+    <t>3/4 Short</t>
+  </si>
+  <si>
+    <t>5/8 Short</t>
+  </si>
+  <si>
+    <t>11/16 Short</t>
+  </si>
+  <si>
+    <t>9/16 Short</t>
+  </si>
+  <si>
+    <t>1/2 Short</t>
+  </si>
+  <si>
+    <t>7/16 Short</t>
+  </si>
+  <si>
+    <t>3/8 Short</t>
+  </si>
+  <si>
+    <t>7/8</t>
+  </si>
+  <si>
+    <t>5/16 Short</t>
+  </si>
+  <si>
+    <t>Standard-Wrench-Ratchet</t>
+  </si>
+  <si>
+    <t>Metric-Wrench-combination</t>
+  </si>
+  <si>
+    <t>24mm</t>
+  </si>
+  <si>
+    <t>27mm</t>
+  </si>
+  <si>
+    <t>22mm</t>
+  </si>
+  <si>
+    <t>21mm</t>
+  </si>
+  <si>
+    <t>19mm</t>
+  </si>
+  <si>
+    <t>18mm</t>
+  </si>
+  <si>
+    <t>17mm</t>
+  </si>
+  <si>
+    <t>16mm</t>
+  </si>
+  <si>
+    <t>15mm</t>
+  </si>
+  <si>
+    <t>14mm</t>
+  </si>
+  <si>
+    <t>13mm</t>
+  </si>
+  <si>
+    <t>12mm</t>
+  </si>
+  <si>
+    <t>11mm</t>
+  </si>
+  <si>
+    <t>10mm</t>
+  </si>
+  <si>
+    <t>Metric-Wrench-Open-End</t>
+  </si>
+  <si>
+    <t>22-24</t>
+  </si>
+  <si>
+    <t>14-17</t>
+  </si>
+  <si>
+    <t>14-12</t>
+  </si>
+  <si>
+    <t>12-10</t>
+  </si>
+  <si>
+    <t>10-8</t>
+  </si>
+  <si>
+    <t>Metric-Wrench-Ratchet-End</t>
+  </si>
+  <si>
+    <t>Box-cutter</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Scissors</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Pliers-Needle-Nose</t>
+  </si>
+  <si>
+    <t>Dark-blue</t>
+  </si>
+  <si>
+    <t>Cyan</t>
+  </si>
+  <si>
+    <t>Standard-blue</t>
+  </si>
+  <si>
+    <t>Yellow-band</t>
+  </si>
+  <si>
+    <t>Pliers-Wire-cutter</t>
+  </si>
+  <si>
+    <t>yellow-band</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>light-blue</t>
+  </si>
+  <si>
+    <t>Jewlers-screwdriver-plastic</t>
+  </si>
+  <si>
+    <t>Yellow-cap</t>
+  </si>
+  <si>
+    <t>Red-cap</t>
+  </si>
+  <si>
+    <t>Jewlers=scewdriver-Silver</t>
+  </si>
+  <si>
+    <t>Phillips</t>
+  </si>
+  <si>
+    <t>Flathead</t>
+  </si>
+  <si>
+    <t>Power-drill</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>Impact-driver</t>
   </si>
 </sst>
 </file>
@@ -498,18 +702,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9CD742-3893-45E5-AF71-D17E57EE27A3}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -520,7 +724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -531,7 +735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -543,9 +747,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f t="shared" ref="A4:A37" si="0">A3+1</f>
+        <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -555,7 +759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -567,7 +771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -579,7 +783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -591,7 +795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -603,7 +807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -615,7 +819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -627,7 +831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -639,7 +843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -652,7 +856,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -665,7 +869,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -678,7 +882,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -691,7 +895,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -704,7 +908,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -717,7 +921,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -729,7 +933,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -741,7 +945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -753,7 +957,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -765,7 +969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -777,7 +981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -789,7 +993,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -801,7 +1005,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -813,7 +1017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -825,97 +1029,1264 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f t="shared" si="0"/>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>36</v>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>50</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>50</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <f t="shared" ref="A68:A131" si="1">A67+1</f>
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>51</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>51</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>51</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>51</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>51</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>51</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>51</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>51</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>51</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>51</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>51</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>66</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>66</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>66</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>66</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>66</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>72</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>72</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>72</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>72</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>72</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>72</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>72</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>72</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>72</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>72</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>72</v>
+      </c>
+      <c r="C102" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>72</v>
+      </c>
+      <c r="C103" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>72</v>
+      </c>
+      <c r="C104" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>72</v>
+      </c>
+      <c r="C105" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>72</v>
+      </c>
+      <c r="C106" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>72</v>
+      </c>
+      <c r="C107" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>72</v>
+      </c>
+      <c r="C108" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>73</v>
+      </c>
+      <c r="C109" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>73</v>
+      </c>
+      <c r="C110" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>73</v>
+      </c>
+      <c r="C111" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>73</v>
+      </c>
+      <c r="C112" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>78</v>
+      </c>
+      <c r="C113" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>78</v>
+      </c>
+      <c r="C114" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>81</v>
+      </c>
+      <c r="C115" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>81</v>
+      </c>
+      <c r="C116" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>81</v>
+      </c>
+      <c r="C117" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>81</v>
+      </c>
+      <c r="C118" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>86</v>
+      </c>
+      <c r="C119" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>81</v>
+      </c>
+      <c r="C120" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>73</v>
+      </c>
+      <c r="C121" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>73</v>
+      </c>
+      <c r="C122" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>91</v>
+      </c>
+      <c r="C123" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>91</v>
+      </c>
+      <c r="C124" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>94</v>
+      </c>
+      <c r="C125" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>94</v>
+      </c>
+      <c r="C126" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>97</v>
+      </c>
+      <c r="C127" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>97</v>
+      </c>
+      <c r="C128" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>97</v>
+      </c>
+      <c r="C129" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>101</v>
+      </c>
+      <c r="C130" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>101</v>
+      </c>
+      <c r="C131" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>